<commit_message>
refactor: 에러 개선 (#noissue)
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/unitTest.xlsx
+++ b/src/main/resources/templates/unitTest.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agsoo\Desktop\KCC\KCC-PMS\src\main\resources\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KCC\final\pms\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FCCE0D9-C864-4ED0-AA8C-6C92FD7D644B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{0350CB31-E14B-4BC0-BCA3-E3AF87F26626}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve"> 테스트 명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -70,62 +69,70 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>테스트 케이스 ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>기능 ID / 기능명</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>사전조건</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테스트 케이스 설명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수행절차 / 테스트 데이터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>예상 결과</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>케이스 작성일자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시험자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테스트 결과</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시험 일자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결과</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>발생한 결함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결과</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테스트 개요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>순번</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사전조건</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>테스트 케이스 설명</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>수행절차 / 테스트 데이터</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>예상 결과</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>케이스 작성일자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>시험자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>테스트 결과</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>시험 일자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>결과</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>발생한 결함</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -161,7 +168,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,8 +181,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -223,14 +236,250 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -241,19 +490,22 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -266,8 +518,113 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -602,285 +959,304 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26813334-C9FA-4A11-9188-E20E98145D2C}">
-  <dimension ref="A1:S13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X9" sqref="S4:X9"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.4140625" customWidth="1"/>
+    <col min="1" max="1" width="5.25" customWidth="1"/>
     <col min="2" max="2" width="8.6640625" customWidth="1"/>
-    <col min="14" max="14" width="10.83203125" customWidth="1"/>
-    <col min="15" max="15" width="10.58203125" customWidth="1"/>
-    <col min="16" max="16" width="11.4140625" customWidth="1"/>
+    <col min="14" max="14" width="7.4140625" customWidth="1"/>
+    <col min="15" max="15" width="7.1640625" customWidth="1"/>
+    <col min="16" max="16" width="8.6640625" customWidth="1"/>
     <col min="17" max="17" width="12.75" customWidth="1"/>
-    <col min="18" max="18" width="13.33203125" customWidth="1"/>
-    <col min="19" max="19" width="12.75" customWidth="1"/>
+    <col min="18" max="18" width="11.75" customWidth="1"/>
+    <col min="19" max="19" width="14.5" customWidth="1"/>
+    <col min="20" max="20" width="8.6640625" customWidth="1"/>
+    <col min="21" max="21" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="11"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
+    <row r="2" spans="1:22" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="12"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="13"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
+    <row r="3" spans="1:22" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="16"/>
+      <c r="U3" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="V3" s="38"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="3" t="s">
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="8"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="22"/>
+      <c r="U4" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="V4" s="40" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A5" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
       <c r="J5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="8"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="24"/>
+      <c r="U5" s="41"/>
+      <c r="V5" s="42"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A6" s="23" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
       <c r="J6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="25"/>
+      <c r="U6" s="41"/>
+      <c r="V6" s="42"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:22" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="25"/>
+      <c r="U7" s="43"/>
+      <c r="V7" s="44"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
+    <row r="8" spans="1:22" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="26"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="29"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+    <row r="9" spans="1:22" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="3" t="s">
+    </row>
+    <row r="10" spans="1:22" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="33"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A11" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="R11" s="18"/>
+      <c r="S11" s="34"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3" t="s">
+    <row r="12" spans="1:22" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="26"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="Q11" s="3" t="s">
+      <c r="R12" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
+      <c r="S12" s="36" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="G13" s="2"/>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="G13" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="28">
+    <mergeCell ref="U3:V3"/>
     <mergeCell ref="A1:Q3"/>
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="N5:Q5"/>
@@ -897,9 +1273,9 @@
     <mergeCell ref="E4:I4"/>
     <mergeCell ref="E5:I5"/>
     <mergeCell ref="A9:D9"/>
-    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="A10:D10"/>
     <mergeCell ref="E9:I9"/>
-    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="E10:H10"/>
     <mergeCell ref="Q11:S11"/>
     <mergeCell ref="P11:P12"/>
     <mergeCell ref="A11:A12"/>
@@ -911,5 +1287,6 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>